<commit_message>
modif systems checklist, modif workflow for v.2.0
</commit_message>
<xml_diff>
--- a/SystemsChecklist.xlsx
+++ b/SystemsChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rad Apdal\OneDrive - yempo\SMS Client Accounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="13_ncr:1_{ED9D96C4-11C2-4E8E-9134-61D03F2F5CEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4387E5AE-A77A-42E2-9DB2-DC291AF21A62}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC671FD-E692-4F0E-9F61-83F6C954A286}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38355" yWindow="1320" windowWidth="13590" windowHeight="14235" activeTab="1" xr2:uid="{D7D68FA9-2D9C-4785-8A4B-D6258F3CA983}"/>
+    <workbookView xWindow="31935" yWindow="1245" windowWidth="13590" windowHeight="14235" activeTab="2" xr2:uid="{D7D68FA9-2D9C-4785-8A4B-D6258F3CA983}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Credentials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
   <si>
     <t>Client Accounts</t>
   </si>
@@ -200,9 +200,6 @@
     <t>PayPal</t>
   </si>
   <si>
-    <t>WooCommerce Settings</t>
-  </si>
-  <si>
     <t>Store Address</t>
   </si>
   <si>
@@ -303,6 +300,69 @@
   </si>
   <si>
     <t>Plugin name</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t>Stripe Email</t>
+  </si>
+  <si>
+    <t>Stripe Sandbox Account</t>
+  </si>
+  <si>
+    <t>General Settings</t>
+  </si>
+  <si>
+    <t>Shipping &amp; Delivery</t>
+  </si>
+  <si>
+    <t>Shipping zones</t>
+  </si>
+  <si>
+    <t>Zone name</t>
+  </si>
+  <si>
+    <t>Zone regions</t>
+  </si>
+  <si>
+    <t>Flat Rate</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>New South Wales, Australia</t>
+  </si>
+  <si>
+    <t>Delivery Options</t>
+  </si>
+  <si>
+    <t>Delivery Range</t>
+  </si>
+  <si>
+    <t>Between 1 and 20 days</t>
+  </si>
+  <si>
+    <t>Delivery days</t>
+  </si>
+  <si>
+    <t>Monday to Friday</t>
+  </si>
+  <si>
+    <t>Maximum delivery days</t>
+  </si>
+  <si>
+    <t>Shipping Method</t>
+  </si>
+  <si>
+    <t>Tax Status</t>
+  </si>
+  <si>
+    <t>Taxable</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -471,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -487,6 +547,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -585,6 +648,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -592,27 +676,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -932,274 +995,274 @@
   <dimension ref="A2:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1212,220 +1275,220 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="17"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -1478,249 +1541,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2B2FE8-D2C7-4A25-B0A0-DC854F35EBC3}">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="44" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="35" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="35" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="35" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="35" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="38" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="44" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="35" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="35" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="35" t="s">
+      <c r="A17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="36" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -1767,70 +1830,70 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="28" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="26" t="s">
+      <c r="F27" s="30"/>
+      <c r="G27" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="27"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="30" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="30" t="s">
+      <c r="D28" s="32"/>
+      <c r="E28" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="30">
+      <c r="F28" s="32"/>
+      <c r="G28" s="31">
         <v>60</v>
       </c>
-      <c r="H28" s="31"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="9"/>
       <c r="D29" s="4"/>
       <c r="E29" s="9"/>
@@ -1839,10 +1902,10 @@
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="25"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -1900,307 +1963,307 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A87E09E-5902-4599-BDEF-BA50D2B91B1A}">
-  <dimension ref="A2:H33"/>
+  <dimension ref="A2:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="48"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="54"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="55"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="52" t="s">
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="48"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19">
         <v>10</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
@@ -2212,99 +2275,322 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="55"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19">
+        <v>10</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="55"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19">
+        <v>90</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="24"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="55"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="23"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="48"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="54"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="20"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="55"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="19"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="74">
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:H37"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A40:H40"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:H25"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:H12"/>
@@ -2313,26 +2599,48 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="D26:H26"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:H21"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D31:H31"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D23:H23"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:H45"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:H49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>